<commit_message>
Deploying to gh-pages from  @ 9433d826b9a1f038641f63a0f702cc48da811bbb 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.2.2.xlsx
+++ b/en/downloads/data-excel/1.2.2.xlsx
@@ -849,9 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -914,6 +912,9 @@
       <c r="H4" s="8">
         <v>2020</v>
       </c>
+      <c r="I4" s="8">
+        <v>2021</v>
+      </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -943,6 +944,9 @@
       </c>
       <c r="H5" s="14">
         <v>42.2</v>
+      </c>
+      <c r="I5" s="14">
+        <v>48.5</v>
       </c>
       <c r="K5" s="37"/>
       <c r="L5" s="15"/>
@@ -964,6 +968,7 @@
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="K6" s="37"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -994,6 +999,9 @@
       <c r="H7" s="34">
         <v>42.5</v>
       </c>
+      <c r="I7" s="34">
+        <v>48.8</v>
+      </c>
       <c r="K7" s="37"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -1023,6 +1031,9 @@
       </c>
       <c r="H8" s="38">
         <v>42</v>
+      </c>
+      <c r="I8" s="38">
+        <v>48.2</v>
       </c>
       <c r="K8" s="37"/>
       <c r="L8" s="15"/>
@@ -1044,6 +1055,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
       <c r="K9" s="37"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1074,6 +1086,9 @@
       <c r="H10" s="38">
         <v>50.9</v>
       </c>
+      <c r="I10" s="38">
+        <v>58.2</v>
+      </c>
       <c r="K10" s="37"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -1104,6 +1119,9 @@
       <c r="H11" s="34">
         <v>36.9</v>
       </c>
+      <c r="I11" s="34">
+        <v>42.4</v>
+      </c>
       <c r="K11" s="37"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
@@ -1133,6 +1151,9 @@
       </c>
       <c r="H12" s="34">
         <v>34.799999999999997</v>
+      </c>
+      <c r="I12" s="34">
+        <v>40.700000000000003</v>
       </c>
       <c r="K12" s="37"/>
     </row>
@@ -1151,6 +1172,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
       <c r="K13" s="37"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
@@ -1181,6 +1203,9 @@
       <c r="H14" s="34">
         <v>30.7</v>
       </c>
+      <c r="I14" s="34">
+        <v>41.5</v>
+      </c>
       <c r="K14" s="37"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -1210,6 +1235,9 @@
       </c>
       <c r="H15" s="34">
         <v>48.8</v>
+      </c>
+      <c r="I15" s="34">
+        <v>52.6</v>
       </c>
       <c r="K15" s="37"/>
       <c r="L15" s="15"/>
@@ -1231,6 +1259,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="16"/>
       <c r="K16" s="37"/>
       <c r="L16" s="15"/>
@@ -1262,6 +1291,9 @@
       <c r="H17" s="34">
         <v>61.1</v>
       </c>
+      <c r="I17" s="34">
+        <v>67.099999999999994</v>
+      </c>
       <c r="K17" s="37"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -1292,6 +1324,9 @@
       <c r="H18" s="34">
         <v>56.7</v>
       </c>
+      <c r="I18" s="34">
+        <v>62</v>
+      </c>
       <c r="K18" s="37"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -1322,6 +1357,9 @@
       <c r="H19" s="34">
         <v>41.6</v>
       </c>
+      <c r="I19" s="34">
+        <v>46.9</v>
+      </c>
       <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1348,6 +1386,9 @@
       </c>
       <c r="H20" s="38">
         <v>49</v>
+      </c>
+      <c r="I20" s="38">
+        <v>55.8</v>
       </c>
       <c r="K20" s="37"/>
       <c r="L20" s="36"/>
@@ -1379,6 +1420,9 @@
       <c r="H21" s="34">
         <v>43.5</v>
       </c>
+      <c r="I21" s="34">
+        <v>42.7</v>
+      </c>
       <c r="K21" s="37"/>
       <c r="L21" s="36"/>
       <c r="M21" s="15"/>
@@ -1409,6 +1453,9 @@
       <c r="H22" s="38">
         <v>33.9</v>
       </c>
+      <c r="I22" s="38">
+        <v>48.3</v>
+      </c>
       <c r="K22" s="37"/>
       <c r="L22" s="36"/>
       <c r="M22" s="15"/>
@@ -1439,6 +1486,9 @@
       <c r="H23" s="38">
         <v>34.6</v>
       </c>
+      <c r="I23" s="38">
+        <v>39.700000000000003</v>
+      </c>
       <c r="K23" s="37"/>
       <c r="L23" s="36"/>
       <c r="M23" s="15"/>
@@ -1469,6 +1519,9 @@
       <c r="H24" s="34">
         <v>23.6</v>
       </c>
+      <c r="I24" s="34">
+        <v>38.1</v>
+      </c>
       <c r="K24" s="37"/>
       <c r="L24" s="36"/>
       <c r="M24" s="15"/>
@@ -1498,6 +1551,9 @@
       </c>
       <c r="H25" s="35">
         <v>35.9</v>
+      </c>
+      <c r="I25" s="35">
+        <v>44.7</v>
       </c>
       <c r="K25" s="37"/>
       <c r="L25" s="36"/>

</xml_diff>